<commit_message>
delete some unuseful files
</commit_message>
<xml_diff>
--- a/results_BSD_10_10.xlsx
+++ b/results_BSD_10_10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhoumengjie/Desktop/route-finder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD3CCFA-46B6-C343-BB07-6D16283EEB21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD3C8FA-6F72-EE49-9EBA-F4EB238D21AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="860" windowWidth="22480" windowHeight="13440" xr2:uid="{DCF972A8-F625-F14C-9F98-97D2BB9C3957}"/>
   </bookViews>
@@ -14941,7 +14941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8D9F61-A412-744D-8F23-E4AC4AB96654}">
   <dimension ref="A1:S94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
       <selection activeCell="O112" sqref="O112"/>
     </sheetView>
   </sheetViews>

</xml_diff>